<commit_message>
add: comparison between ideal and hardware
</commit_message>
<xml_diff>
--- a/Simulasi_Vector/Weight dan bias hasil training.xlsx
+++ b/Simulasi_Vector/Weight dan bias hasil training.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITB\Semester V\Perancangan Sistem VLSI\UAS\github\UAS_VLSI_LEVEL1-OKINAWA\Simulasi_Vector\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Okinawa\UAS_VLSI_LEVEL1-OKINAWA\Simulasi_Vector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C414E348-AA4A-4738-B5B5-E19B5B67B620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B707F32-80AA-4AD2-AC2E-B46034038205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C54F6822-D4A8-46D5-BD9B-B2A846AAD251}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>Wd2</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Cross</t>
   </si>
   <si>
-    <t xml:space="preserve">Perbandingan data </t>
-  </si>
-  <si>
     <t>Ideal</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t>Input</t>
   </si>
   <si>
-    <t>[0,1]</t>
-  </si>
-  <si>
     <t xml:space="preserve">skor : </t>
   </si>
   <si>
@@ -91,6 +85,27 @@
   </si>
   <si>
     <t>PWQ (tanh)</t>
+  </si>
+  <si>
+    <t>[0,1] cross</t>
+  </si>
+  <si>
+    <t>[1,0] cross</t>
+  </si>
+  <si>
+    <t>Perbandingan data (xfake keluaran generator)</t>
+  </si>
+  <si>
+    <t>[0,1] circle</t>
+  </si>
+  <si>
+    <t>[1,0] circle</t>
+  </si>
+  <si>
+    <t>Perbandingan data (keluaran discriminator)</t>
+  </si>
+  <si>
+    <t>PWQ(tanh) + PWL (Sigmoid)</t>
   </si>
 </sst>
 </file>
@@ -448,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05913C57-9BC5-4BEF-9885-2849EB63E124}">
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:O78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="64" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42:F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1064,29 +1079,49 @@
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B40" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2" t="s">
-        <v>14</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M40" s="2"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E41" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F41" s="2"/>
+      <c r="H41" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B42" s="1">
@@ -1102,8 +1137,20 @@
         <v>-0.97781284255234102</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="H42" s="2">
+        <v>0.470764938554386</v>
+      </c>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2">
+        <v>0.467146543573427</v>
+      </c>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M42" s="2"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B43" s="1">
@@ -1119,6 +1166,12 @@
         <v>0.97988784299996501</v>
       </c>
       <c r="F43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B44" s="1">
@@ -1134,6 +1187,12 @@
         <v>-0.97799124990097697</v>
       </c>
       <c r="F44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B45" s="1">
@@ -1149,6 +1208,12 @@
         <v>0.97929738027313595</v>
       </c>
       <c r="F45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B46" s="1">
@@ -1164,6 +1229,12 @@
         <v>0.97848811244893397</v>
       </c>
       <c r="F46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B47" s="1">
@@ -1179,6 +1250,12 @@
         <v>0.97892990008482905</v>
       </c>
       <c r="F47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B48" s="1">
@@ -1194,8 +1271,14 @@
         <v>-0.97785900318604402</v>
       </c>
       <c r="F48" s="2"/>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B49" s="1">
         <v>0.978931419627038</v>
       </c>
@@ -1209,9 +1292,17 @@
         <v>0.97802528019285395</v>
       </c>
       <c r="F49" s="2"/>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B50" s="1"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B50" s="1">
+        <v>-0.98108158968943504</v>
+      </c>
       <c r="C50" s="1">
         <v>-0.98135952650237002</v>
       </c>
@@ -1222,27 +1313,481 @@
         <v>-0.97979759988389203</v>
       </c>
       <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B51" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F51" s="2"/>
+      <c r="H51" s="2">
+        <v>0.47107202254688402</v>
+      </c>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2">
+        <v>0.46739828818349</v>
+      </c>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M51" s="2"/>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B52">
+        <v>-0.97868028849224198</v>
+      </c>
+      <c r="E52" s="1">
+        <v>-0.97783583064508095</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B53">
+        <v>0.98122731568354904</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0.97992046254868803</v>
+      </c>
+      <c r="F53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B54">
+        <v>-0.97936820672860903</v>
+      </c>
+      <c r="E54" s="1">
+        <v>-0.97835316255938398</v>
+      </c>
+      <c r="F54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B55">
+        <v>0.98029939051586901</v>
+      </c>
+      <c r="E55" s="1">
+        <v>0.97915203110764903</v>
+      </c>
+      <c r="F55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+    </row>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B56">
+        <v>0.97979857599756703</v>
+      </c>
+      <c r="E56" s="1">
+        <v>0.97871088848453902</v>
+      </c>
+      <c r="F56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="2"/>
+    </row>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B57">
+        <v>0.97979113321798805</v>
+      </c>
+      <c r="E57" s="1">
+        <v>0.97873998805777995</v>
+      </c>
+      <c r="F57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+      <c r="M57" s="2"/>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B58">
+        <v>-0.97894082142066097</v>
+      </c>
+      <c r="E58" s="1">
+        <v>-0.97802358155525404</v>
+      </c>
+      <c r="F58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+      <c r="M58" s="2"/>
+    </row>
+    <row r="59" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B59">
+        <v>0.979050434209914</v>
+      </c>
+      <c r="E59" s="1">
+        <v>0.97811740815373105</v>
+      </c>
+      <c r="F59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+    </row>
+    <row r="60" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B60">
+        <v>-0.98118862643534899</v>
+      </c>
+      <c r="E60" s="1">
+        <v>-0.97988609234058599</v>
+      </c>
+      <c r="F60" s="2"/>
+      <c r="H60" s="2">
+        <v>0.470996508933822</v>
+      </c>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2">
+        <v>0.47087036808694599</v>
+      </c>
+      <c r="K60" s="2"/>
+      <c r="L60" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M60" s="2"/>
+    </row>
+    <row r="61" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B61">
+        <v>0.97730843041321103</v>
+      </c>
+      <c r="E61" s="1">
+        <v>0.97689121961593595</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+      <c r="M61" s="2"/>
+    </row>
+    <row r="62" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B62">
+        <v>0.97850035024318305</v>
+      </c>
+      <c r="E62" s="1">
+        <v>0.977819263935089</v>
+      </c>
+      <c r="F62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+      <c r="M62" s="2"/>
+    </row>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B63">
+        <v>0.97705339412759595</v>
+      </c>
+      <c r="E63" s="1">
+        <v>0.97672259807586703</v>
+      </c>
+      <c r="F63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+      <c r="M63" s="2"/>
+    </row>
+    <row r="64" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B64">
+        <v>0.97889631573253399</v>
+      </c>
+      <c r="E64" s="1">
+        <v>0.97814095020294201</v>
+      </c>
+      <c r="F64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+      <c r="M64" s="2"/>
+    </row>
+    <row r="65" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B65">
+        <v>-0.97932019701578099</v>
+      </c>
+      <c r="E65" s="1">
+        <v>-0.978462934494019</v>
+      </c>
+      <c r="F65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+      <c r="M65" s="2"/>
+    </row>
+    <row r="66" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B66">
+        <v>0.97967833912446001</v>
+      </c>
+      <c r="E66" s="1">
+        <v>0.97876471281051602</v>
+      </c>
+      <c r="F66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2"/>
+      <c r="K66" s="2"/>
+      <c r="L66" s="2"/>
+      <c r="M66" s="2"/>
+    </row>
+    <row r="67" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B67">
+        <v>0.97892031512594602</v>
+      </c>
+      <c r="E67" s="1">
+        <v>0.97814756631851196</v>
+      </c>
+      <c r="F67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2"/>
+      <c r="K67" s="2"/>
+      <c r="L67" s="2"/>
+      <c r="M67" s="2"/>
+    </row>
+    <row r="68" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B68">
+        <v>0.98046374759541999</v>
+      </c>
+      <c r="E68" s="1">
+        <v>0.97939556837081898</v>
+      </c>
+      <c r="F68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
+      <c r="M68" s="2"/>
+    </row>
+    <row r="69" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B69">
+        <v>0.97895422239492103</v>
+      </c>
+      <c r="E69" s="1">
+        <v>0.97817534208297696</v>
+      </c>
+      <c r="F69" s="2"/>
+      <c r="H69" s="2">
+        <v>0.47080308116633002</v>
+      </c>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2">
+        <v>0.470775017264912</v>
+      </c>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M69" s="2"/>
+    </row>
+    <row r="70" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B70">
+        <v>0.97703604095575403</v>
+      </c>
+      <c r="E70" s="1">
+        <v>0.97669219970703103</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2"/>
+      <c r="K70" s="2"/>
+      <c r="L70" s="2"/>
+      <c r="M70" s="2"/>
+    </row>
+    <row r="71" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B71">
+        <v>0.97806477277616999</v>
+      </c>
+      <c r="E71" s="1">
+        <v>0.97748142480850198</v>
+      </c>
+      <c r="F71" s="2"/>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="2"/>
+      <c r="K71" s="2"/>
+      <c r="L71" s="2"/>
+      <c r="M71" s="2"/>
+    </row>
+    <row r="72" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B72">
+        <v>0.97681122053494496</v>
+      </c>
+      <c r="E72" s="1">
+        <v>0.97655534744262695</v>
+      </c>
+      <c r="F72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
+      <c r="J72" s="2"/>
+      <c r="K72" s="2"/>
+      <c r="L72" s="2"/>
+      <c r="M72" s="2"/>
+    </row>
+    <row r="73" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B73">
+        <v>0.97901343466412905</v>
+      </c>
+      <c r="E73" s="1">
+        <v>0.97826117277145397</v>
+      </c>
+      <c r="F73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
+      <c r="K73" s="2"/>
+      <c r="L73" s="2"/>
+      <c r="M73" s="2"/>
+    </row>
+    <row r="74" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B74">
+        <v>-0.979210132223582</v>
+      </c>
+      <c r="E74" s="1">
+        <v>-0.97838181257247903</v>
+      </c>
+      <c r="F74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2"/>
+      <c r="K74" s="2"/>
+      <c r="L74" s="2"/>
+      <c r="M74" s="2"/>
+    </row>
+    <row r="75" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B75">
+        <v>0.97987911658029803</v>
+      </c>
+      <c r="E75" s="1">
+        <v>0.97895503044128396</v>
+      </c>
+      <c r="F75" s="2"/>
+      <c r="H75" s="2"/>
+      <c r="I75" s="2"/>
+      <c r="J75" s="2"/>
+      <c r="K75" s="2"/>
+      <c r="L75" s="2"/>
+      <c r="M75" s="2"/>
+    </row>
+    <row r="76" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B76">
+        <v>0.97845001803704401</v>
+      </c>
+      <c r="E76" s="1">
+        <v>0.97777229547500599</v>
+      </c>
+      <c r="F76" s="2"/>
+      <c r="H76" s="2"/>
+      <c r="I76" s="2"/>
+      <c r="J76" s="2"/>
+      <c r="K76" s="2"/>
+      <c r="L76" s="2"/>
+      <c r="M76" s="2"/>
+    </row>
+    <row r="77" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B77">
+        <v>0.98078457113886097</v>
+      </c>
+      <c r="E77" s="1">
+        <v>0.97969591617584195</v>
+      </c>
+      <c r="F77" s="2"/>
+      <c r="H77" s="2"/>
+      <c r="I77" s="2"/>
+      <c r="J77" s="2"/>
+      <c r="K77" s="2"/>
+      <c r="L77" s="2"/>
+      <c r="M77" s="2"/>
+    </row>
+    <row r="78" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B78">
+        <v>0.97934031696857804</v>
+      </c>
+      <c r="E78" s="1">
+        <v>0.97852188348770097</v>
+      </c>
+      <c r="F78" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="22">
+    <mergeCell ref="H60:I68"/>
+    <mergeCell ref="J60:K68"/>
+    <mergeCell ref="H69:I77"/>
+    <mergeCell ref="J69:K77"/>
+    <mergeCell ref="L69:M77"/>
+    <mergeCell ref="L60:M68"/>
+    <mergeCell ref="H51:I59"/>
+    <mergeCell ref="J51:K59"/>
+    <mergeCell ref="L42:M50"/>
+    <mergeCell ref="L51:M59"/>
+    <mergeCell ref="H42:I50"/>
+    <mergeCell ref="J42:K50"/>
+    <mergeCell ref="F70:F78"/>
+    <mergeCell ref="H40:K40"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="L40:M41"/>
     <mergeCell ref="F40:F41"/>
     <mergeCell ref="B40:E40"/>
     <mergeCell ref="F42:F51"/>
+    <mergeCell ref="F52:F60"/>
+    <mergeCell ref="F61:F69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add: error between software and hardware
</commit_message>
<xml_diff>
--- a/Simulasi_Vector/Weight dan bias hasil training.xlsx
+++ b/Simulasi_Vector/Weight dan bias hasil training.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Okinawa\UAS_VLSI_LEVEL1-OKINAWA\Simulasi_Vector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018E2BAD-E6EC-4862-8B9E-7F2821E9C48A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959F3AE9-3331-41E0-8FCD-41AC79EFCBDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C54F6822-D4A8-46D5-BD9B-B2A846AAD251}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="26">
   <si>
     <t>Wd2</t>
   </si>
@@ -100,6 +100,18 @@
   </si>
   <si>
     <t>Data Keluaran Discriminator</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>Error (%)</t>
+  </si>
+  <si>
+    <t>Error(%)</t>
   </si>
 </sst>
 </file>
@@ -464,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05913C57-9BC5-4BEF-9885-2849EB63E124}">
-  <dimension ref="A1:T103"/>
+  <dimension ref="A1:T147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F41" zoomScale="64" workbookViewId="0">
-      <selection activeCell="P58" sqref="P58:R58"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="63" workbookViewId="0">
+      <selection activeCell="C109" sqref="C109:G117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1511,7 +1523,7 @@
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
       <c r="P58" s="4">
-        <v>0.470996508933822</v>
+        <v>0.47087036808694599</v>
       </c>
       <c r="Q58" s="4"/>
       <c r="R58" s="4"/>
@@ -1537,7 +1549,7 @@
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
       <c r="P59" s="4">
-        <v>0.47080308116633002</v>
+        <v>0.470775017264912</v>
       </c>
       <c r="Q59" s="4"/>
       <c r="R59" s="4"/>
@@ -2459,8 +2471,1042 @@
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
     </row>
+    <row r="109" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C109" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D109" s="2"/>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2"/>
+      <c r="G109" s="2"/>
+      <c r="H109" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="110" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C110" t="s">
+        <v>24</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G110" s="2"/>
+      <c r="H110" s="2"/>
+      <c r="L110" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M110" s="2"/>
+      <c r="N110" s="2"/>
+      <c r="O110" s="2"/>
+      <c r="P110" s="2"/>
+      <c r="Q110" s="2"/>
+      <c r="R110" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="S110" s="2"/>
+    </row>
+    <row r="111" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C111">
+        <f>ABS((F111-D111)*100/F111)</f>
+        <v>2.0477121180605566E-2</v>
+      </c>
+      <c r="D111" s="2">
+        <v>-0.97761261463165205</v>
+      </c>
+      <c r="E111" s="2"/>
+      <c r="F111" s="2">
+        <v>-0.97781284255234102</v>
+      </c>
+      <c r="G111" s="2"/>
+      <c r="H111" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L111" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M111" s="2"/>
+      <c r="N111" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O111" s="2"/>
+      <c r="P111" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q111" s="2"/>
+      <c r="R111" s="2"/>
+      <c r="S111" s="2"/>
+    </row>
+    <row r="112" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C112">
+        <f t="shared" ref="C112:C147" si="0">ABS((F112-D112)*100/F112)</f>
+        <v>2.8899382444319967E-2</v>
+      </c>
+      <c r="D112" s="2">
+        <v>0.97960466146469105</v>
+      </c>
+      <c r="E112" s="2"/>
+      <c r="F112" s="2">
+        <v>0.97988784299996501</v>
+      </c>
+      <c r="G112" s="2"/>
+      <c r="H112" s="2"/>
+      <c r="L112" s="2">
+        <f>ABS((P112-N112)*100/P112)</f>
+        <v>0.69513367261435921</v>
+      </c>
+      <c r="M112" s="2"/>
+      <c r="N112" s="2">
+        <v>0.47039383649826</v>
+      </c>
+      <c r="O112" s="2"/>
+      <c r="P112" s="2">
+        <v>0.467146543573427</v>
+      </c>
+      <c r="Q112" s="2"/>
+      <c r="R112" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="S112" s="2"/>
+    </row>
+    <row r="113" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C113">
+        <f t="shared" si="0"/>
+        <v>1.1996887154237097E-2</v>
+      </c>
+      <c r="D113" s="2">
+        <v>-0.97787392139434803</v>
+      </c>
+      <c r="E113" s="2"/>
+      <c r="F113" s="2">
+        <v>-0.97799124990097697</v>
+      </c>
+      <c r="G113" s="2"/>
+      <c r="H113" s="2"/>
+      <c r="L113" s="2"/>
+      <c r="M113" s="2"/>
+      <c r="N113" s="2"/>
+      <c r="O113" s="2"/>
+      <c r="P113" s="2"/>
+      <c r="Q113" s="2"/>
+      <c r="R113" s="2"/>
+      <c r="S113" s="2"/>
+    </row>
+    <row r="114" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C114">
+        <f t="shared" si="0"/>
+        <v>2.3546588354356884E-2</v>
+      </c>
+      <c r="D114" s="2">
+        <v>0.97906678915023804</v>
+      </c>
+      <c r="E114" s="2"/>
+      <c r="F114" s="2">
+        <v>0.97929738027313595</v>
+      </c>
+      <c r="G114" s="2"/>
+      <c r="H114" s="2"/>
+      <c r="L114" s="2"/>
+      <c r="M114" s="2"/>
+      <c r="N114" s="2"/>
+      <c r="O114" s="2"/>
+      <c r="P114" s="2"/>
+      <c r="Q114" s="2"/>
+      <c r="R114" s="2"/>
+      <c r="S114" s="2"/>
+    </row>
+    <row r="115" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C115">
+        <f t="shared" si="0"/>
+        <v>2.6756420578139432E-2</v>
+      </c>
+      <c r="D115" s="2">
+        <v>0.97822630405426003</v>
+      </c>
+      <c r="E115" s="2"/>
+      <c r="F115" s="2">
+        <v>0.97848811244893397</v>
+      </c>
+      <c r="G115" s="2"/>
+      <c r="H115" s="2"/>
+      <c r="L115" s="2"/>
+      <c r="M115" s="2"/>
+      <c r="N115" s="2"/>
+      <c r="O115" s="2"/>
+      <c r="P115" s="2"/>
+      <c r="Q115" s="2"/>
+      <c r="R115" s="2"/>
+      <c r="S115" s="2"/>
+    </row>
+    <row r="116" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C116">
+        <f t="shared" si="0"/>
+        <v>2.0594499386885966E-2</v>
+      </c>
+      <c r="D116" s="2">
+        <v>0.97872829437255804</v>
+      </c>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2">
+        <v>0.97892990008482905</v>
+      </c>
+      <c r="G116" s="2"/>
+      <c r="H116" s="2"/>
+      <c r="L116" s="2"/>
+      <c r="M116" s="2"/>
+      <c r="N116" s="2"/>
+      <c r="O116" s="2"/>
+      <c r="P116" s="2"/>
+      <c r="Q116" s="2"/>
+      <c r="R116" s="2"/>
+      <c r="S116" s="2"/>
+    </row>
+    <row r="117" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C117">
+        <f t="shared" si="0"/>
+        <v>2.242941415372111E-2</v>
+      </c>
+      <c r="D117" s="2">
+        <v>-0.97763967514037997</v>
+      </c>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2">
+        <v>-0.97785900318604402</v>
+      </c>
+      <c r="G117" s="2"/>
+      <c r="H117" s="2"/>
+      <c r="L117" s="2"/>
+      <c r="M117" s="2"/>
+      <c r="N117" s="2"/>
+      <c r="O117" s="2"/>
+      <c r="P117" s="2"/>
+      <c r="Q117" s="2"/>
+      <c r="R117" s="2"/>
+      <c r="S117" s="2"/>
+    </row>
+    <row r="118" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C118">
+        <f t="shared" si="0"/>
+        <v>2.2502787851101994E-2</v>
+      </c>
+      <c r="D118" s="2">
+        <v>0.97780519723892201</v>
+      </c>
+      <c r="E118" s="2"/>
+      <c r="F118" s="2">
+        <v>0.97802528019285395</v>
+      </c>
+      <c r="G118" s="2"/>
+      <c r="H118" s="2"/>
+      <c r="L118" s="2"/>
+      <c r="M118" s="2"/>
+      <c r="N118" s="2"/>
+      <c r="O118" s="2"/>
+      <c r="P118" s="2"/>
+      <c r="Q118" s="2"/>
+      <c r="R118" s="2"/>
+      <c r="S118" s="2"/>
+    </row>
+    <row r="119" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C119" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2093540328238901E-2</v>
+      </c>
+      <c r="D119" s="2">
+        <v>-0.97967910766601496</v>
+      </c>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2">
+        <v>-0.97979759988389203</v>
+      </c>
+      <c r="G119" s="2"/>
+      <c r="H119" s="2"/>
+      <c r="L119" s="2"/>
+      <c r="M119" s="2"/>
+      <c r="N119" s="2"/>
+      <c r="O119" s="2"/>
+      <c r="P119" s="2"/>
+      <c r="Q119" s="2"/>
+      <c r="R119" s="2"/>
+      <c r="S119" s="2"/>
+    </row>
+    <row r="120" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C120" s="2"/>
+      <c r="D120" s="2"/>
+      <c r="E120" s="2"/>
+      <c r="F120" s="2"/>
+      <c r="G120" s="2"/>
+      <c r="H120" s="2"/>
+      <c r="L120" s="2"/>
+      <c r="M120" s="2"/>
+      <c r="N120" s="2"/>
+      <c r="O120" s="2"/>
+      <c r="P120" s="2"/>
+      <c r="Q120" s="2"/>
+      <c r="R120" s="2"/>
+      <c r="S120" s="2"/>
+    </row>
+    <row r="121" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C121">
+        <f t="shared" si="0"/>
+        <v>5.3698493291368266E-3</v>
+      </c>
+      <c r="D121" s="2">
+        <v>-0.977783322334289</v>
+      </c>
+      <c r="E121" s="2"/>
+      <c r="F121" s="2">
+        <v>-0.97783583064508095</v>
+      </c>
+      <c r="G121" s="2"/>
+      <c r="H121" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L121" s="2">
+        <f>ABS((P121-N121)*100/P121)</f>
+        <v>0.80103071274946891</v>
+      </c>
+      <c r="M121" s="2"/>
+      <c r="N121" s="2">
+        <v>0.47114229202270502</v>
+      </c>
+      <c r="O121" s="2"/>
+      <c r="P121" s="2">
+        <v>0.46739828818349</v>
+      </c>
+      <c r="Q121" s="2"/>
+      <c r="R121" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="S121" s="2"/>
+    </row>
+    <row r="122" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C122">
+        <f t="shared" si="0"/>
+        <v>1.265949089708179E-2</v>
+      </c>
+      <c r="D122" s="2">
+        <v>0.97979640960693304</v>
+      </c>
+      <c r="E122" s="2"/>
+      <c r="F122" s="2">
+        <v>0.97992046254868803</v>
+      </c>
+      <c r="G122" s="2"/>
+      <c r="H122" s="2"/>
+      <c r="L122" s="2"/>
+      <c r="M122" s="2"/>
+      <c r="N122" s="2"/>
+      <c r="O122" s="2"/>
+      <c r="P122" s="2"/>
+      <c r="Q122" s="2"/>
+      <c r="R122" s="2"/>
+      <c r="S122" s="2"/>
+    </row>
+    <row r="123" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C123">
+        <f t="shared" si="0"/>
+        <v>3.858002666725277E-5</v>
+      </c>
+      <c r="D123" s="2">
+        <v>-0.97835278511047297</v>
+      </c>
+      <c r="E123" s="2"/>
+      <c r="F123" s="2">
+        <v>-0.97835316255938398</v>
+      </c>
+      <c r="G123" s="2"/>
+      <c r="H123" s="2"/>
+      <c r="L123" s="2"/>
+      <c r="M123" s="2"/>
+      <c r="N123" s="2"/>
+      <c r="O123" s="2"/>
+      <c r="P123" s="2"/>
+      <c r="Q123" s="2"/>
+      <c r="R123" s="2"/>
+      <c r="S123" s="2"/>
+    </row>
+    <row r="124" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C124">
+        <f t="shared" si="0"/>
+        <v>4.8402093314820586E-3</v>
+      </c>
+      <c r="D124" s="2">
+        <v>0.97910463809966997</v>
+      </c>
+      <c r="E124" s="2"/>
+      <c r="F124" s="2">
+        <v>0.97915203110764903</v>
+      </c>
+      <c r="G124" s="2"/>
+      <c r="H124" s="2"/>
+      <c r="L124" s="2"/>
+      <c r="M124" s="2"/>
+      <c r="N124" s="2"/>
+      <c r="O124" s="2"/>
+      <c r="P124" s="2"/>
+      <c r="Q124" s="2"/>
+      <c r="R124" s="2"/>
+      <c r="S124" s="2"/>
+    </row>
+    <row r="125" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C125">
+        <f t="shared" si="0"/>
+        <v>6.6502724262927472E-3</v>
+      </c>
+      <c r="D125" s="2">
+        <v>0.97864580154418901</v>
+      </c>
+      <c r="E125" s="2"/>
+      <c r="F125" s="2">
+        <v>0.97871088848453902</v>
+      </c>
+      <c r="G125" s="2"/>
+      <c r="H125" s="2"/>
+      <c r="L125" s="2"/>
+      <c r="M125" s="2"/>
+      <c r="N125" s="2"/>
+      <c r="O125" s="2"/>
+      <c r="P125" s="2"/>
+      <c r="Q125" s="2"/>
+      <c r="R125" s="2"/>
+      <c r="S125" s="2"/>
+    </row>
+    <row r="126" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C126">
+        <f t="shared" si="0"/>
+        <v>4.3980759853709337E-3</v>
+      </c>
+      <c r="D126" s="2">
+        <v>0.97869694232940596</v>
+      </c>
+      <c r="E126" s="2"/>
+      <c r="F126" s="2">
+        <v>0.97873998805777995</v>
+      </c>
+      <c r="G126" s="2"/>
+      <c r="H126" s="2"/>
+      <c r="L126" s="2"/>
+      <c r="M126" s="2"/>
+      <c r="N126" s="2"/>
+      <c r="O126" s="2"/>
+      <c r="P126" s="2"/>
+      <c r="Q126" s="2"/>
+      <c r="R126" s="2"/>
+      <c r="S126" s="2"/>
+    </row>
+    <row r="127" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C127">
+        <f t="shared" si="0"/>
+        <v>3.9301602210749095E-3</v>
+      </c>
+      <c r="D127" s="2">
+        <v>-0.97798514366149902</v>
+      </c>
+      <c r="E127" s="2"/>
+      <c r="F127" s="2">
+        <v>-0.97802358155525404</v>
+      </c>
+      <c r="G127" s="2"/>
+      <c r="H127" s="2"/>
+      <c r="L127" s="2"/>
+      <c r="M127" s="2"/>
+      <c r="N127" s="2"/>
+      <c r="O127" s="2"/>
+      <c r="P127" s="2"/>
+      <c r="Q127" s="2"/>
+      <c r="R127" s="2"/>
+      <c r="S127" s="2"/>
+    </row>
+    <row r="128" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C128">
+        <f t="shared" si="0"/>
+        <v>5.7771171693713859E-3</v>
+      </c>
+      <c r="D128" s="2">
+        <v>0.97806090116500799</v>
+      </c>
+      <c r="E128" s="2"/>
+      <c r="F128" s="2">
+        <v>0.97811740815373105</v>
+      </c>
+      <c r="G128" s="2"/>
+      <c r="H128" s="2"/>
+      <c r="L128" s="2"/>
+      <c r="M128" s="2"/>
+      <c r="N128" s="2"/>
+      <c r="O128" s="2"/>
+      <c r="P128" s="2"/>
+      <c r="Q128" s="2"/>
+      <c r="R128" s="2"/>
+      <c r="S128" s="2"/>
+    </row>
+    <row r="129" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C129">
+        <f t="shared" si="0"/>
+        <v>3.7940580431080793E-4</v>
+      </c>
+      <c r="D129" s="2">
+        <v>-0.97988981008529596</v>
+      </c>
+      <c r="E129" s="2"/>
+      <c r="F129" s="2">
+        <v>-0.97988609234058599</v>
+      </c>
+      <c r="G129" s="2"/>
+      <c r="H129" s="2"/>
+      <c r="L129" s="2"/>
+      <c r="M129" s="2"/>
+      <c r="N129" s="2"/>
+      <c r="O129" s="2"/>
+      <c r="P129" s="2"/>
+      <c r="Q129" s="2"/>
+      <c r="R129" s="2"/>
+      <c r="S129" s="2"/>
+    </row>
+    <row r="130" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C130">
+        <f t="shared" si="0"/>
+        <v>2.7822665893749029E-3</v>
+      </c>
+      <c r="D130" s="2">
+        <v>0.97686403989791804</v>
+      </c>
+      <c r="E130" s="2"/>
+      <c r="F130" s="2">
+        <v>0.97689121961593595</v>
+      </c>
+      <c r="G130" s="2"/>
+      <c r="H130" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L130" s="2">
+        <f>ABS((P130-N130)*100/P130)</f>
+        <v>0.9182291277366218</v>
+      </c>
+      <c r="M130" s="2"/>
+      <c r="N130" s="2">
+        <v>0.47519403696060097</v>
+      </c>
+      <c r="O130" s="2"/>
+      <c r="P130" s="2">
+        <v>0.47087036808694599</v>
+      </c>
+      <c r="Q130" s="2"/>
+      <c r="R130" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S130" s="2"/>
+    </row>
+    <row r="131" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C131">
+        <f t="shared" si="0"/>
+        <v>3.3770017040902294E-3</v>
+      </c>
+      <c r="D131" s="2">
+        <v>0.97778624296188299</v>
+      </c>
+      <c r="E131" s="2"/>
+      <c r="F131" s="2">
+        <v>0.977819263935089</v>
+      </c>
+      <c r="G131" s="2"/>
+      <c r="H131" s="2"/>
+      <c r="L131" s="2"/>
+      <c r="M131" s="2"/>
+      <c r="N131" s="2"/>
+      <c r="O131" s="2"/>
+      <c r="P131" s="2"/>
+      <c r="Q131" s="2"/>
+      <c r="R131" s="2"/>
+      <c r="S131" s="2"/>
+    </row>
+    <row r="132" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C132">
+        <f t="shared" si="0"/>
+        <v>2.9353097997888425E-3</v>
+      </c>
+      <c r="D132" s="2">
+        <v>0.97669392824172896</v>
+      </c>
+      <c r="E132" s="2"/>
+      <c r="F132" s="2">
+        <v>0.97672259807586703</v>
+      </c>
+      <c r="G132" s="2"/>
+      <c r="H132" s="2"/>
+      <c r="L132" s="2"/>
+      <c r="M132" s="2"/>
+      <c r="N132" s="2"/>
+      <c r="O132" s="2"/>
+      <c r="P132" s="2"/>
+      <c r="Q132" s="2"/>
+      <c r="R132" s="2"/>
+      <c r="S132" s="2"/>
+    </row>
+    <row r="133" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C133">
+        <f t="shared" si="0"/>
+        <v>4.1254120384877331E-3</v>
+      </c>
+      <c r="D133" s="2">
+        <v>0.97810059785842896</v>
+      </c>
+      <c r="E133" s="2"/>
+      <c r="F133" s="2">
+        <v>0.97814095020294201</v>
+      </c>
+      <c r="G133" s="2"/>
+      <c r="H133" s="2"/>
+      <c r="L133" s="2"/>
+      <c r="M133" s="2"/>
+      <c r="N133" s="2"/>
+      <c r="O133" s="2"/>
+      <c r="P133" s="2"/>
+      <c r="Q133" s="2"/>
+      <c r="R133" s="2"/>
+      <c r="S133" s="2"/>
+    </row>
+    <row r="134" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C134">
+        <f t="shared" si="0"/>
+        <v>3.1755828684065381E-2</v>
+      </c>
+      <c r="D134" s="2">
+        <v>-0.978152215480804</v>
+      </c>
+      <c r="E134" s="2"/>
+      <c r="F134" s="2">
+        <v>-0.978462934494019</v>
+      </c>
+      <c r="G134" s="2"/>
+      <c r="H134" s="2"/>
+      <c r="L134" s="2"/>
+      <c r="M134" s="2"/>
+      <c r="N134" s="2"/>
+      <c r="O134" s="2"/>
+      <c r="P134" s="2"/>
+      <c r="Q134" s="2"/>
+      <c r="R134" s="2"/>
+      <c r="S134" s="2"/>
+    </row>
+    <row r="135" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C135">
+        <f t="shared" si="0"/>
+        <v>5.1702255661285083E-3</v>
+      </c>
+      <c r="D135" s="2">
+        <v>0.97871410846710205</v>
+      </c>
+      <c r="E135" s="2"/>
+      <c r="F135" s="2">
+        <v>0.97876471281051602</v>
+      </c>
+      <c r="G135" s="2"/>
+      <c r="H135" s="2"/>
+      <c r="L135" s="2"/>
+      <c r="M135" s="2"/>
+      <c r="N135" s="2"/>
+      <c r="O135" s="2"/>
+      <c r="P135" s="2"/>
+      <c r="Q135" s="2"/>
+      <c r="R135" s="2"/>
+      <c r="S135" s="2"/>
+    </row>
+    <row r="136" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C136">
+        <f t="shared" si="0"/>
+        <v>3.3149320076481248E-3</v>
+      </c>
+      <c r="D136" s="2">
+        <v>0.97811514139175404</v>
+      </c>
+      <c r="E136" s="2"/>
+      <c r="F136" s="2">
+        <v>0.97814756631851196</v>
+      </c>
+      <c r="G136" s="2"/>
+      <c r="H136" s="2"/>
+      <c r="L136" s="2"/>
+      <c r="M136" s="2"/>
+      <c r="N136" s="2"/>
+      <c r="O136" s="2"/>
+      <c r="P136" s="2"/>
+      <c r="Q136" s="2"/>
+      <c r="R136" s="2"/>
+      <c r="S136" s="2"/>
+    </row>
+    <row r="137" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C137">
+        <f t="shared" si="0"/>
+        <v>5.2277538836651158E-3</v>
+      </c>
+      <c r="D137" s="2">
+        <v>0.97934436798095703</v>
+      </c>
+      <c r="E137" s="2"/>
+      <c r="F137" s="2">
+        <v>0.97939556837081898</v>
+      </c>
+      <c r="G137" s="2"/>
+      <c r="H137" s="2"/>
+      <c r="L137" s="2"/>
+      <c r="M137" s="2"/>
+      <c r="N137" s="2"/>
+      <c r="O137" s="2"/>
+      <c r="P137" s="2"/>
+      <c r="Q137" s="2"/>
+      <c r="R137" s="2"/>
+      <c r="S137" s="2"/>
+    </row>
+    <row r="138" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C138">
+        <f t="shared" si="0"/>
+        <v>0.11951087373462976</v>
+      </c>
+      <c r="D138" s="2">
+        <v>0.97934436798095703</v>
+      </c>
+      <c r="E138" s="2"/>
+      <c r="F138" s="2">
+        <v>0.97817534208297696</v>
+      </c>
+      <c r="G138" s="2"/>
+      <c r="H138" s="2"/>
+      <c r="L138" s="2"/>
+      <c r="M138" s="2"/>
+      <c r="N138" s="2"/>
+      <c r="O138" s="2"/>
+      <c r="P138" s="2"/>
+      <c r="Q138" s="2"/>
+      <c r="R138" s="2"/>
+      <c r="S138" s="2"/>
+    </row>
+    <row r="139" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C139">
+        <f t="shared" si="0"/>
+        <v>3.0208390292141706E-3</v>
+      </c>
+      <c r="D139" s="2">
+        <v>0.97666269540786699</v>
+      </c>
+      <c r="E139" s="2"/>
+      <c r="F139" s="2">
+        <v>0.97669219970703103</v>
+      </c>
+      <c r="G139" s="2"/>
+      <c r="H139" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L139" s="2">
+        <f>ABS((P139-N139)*100/P139)</f>
+        <v>0.92619806928547832</v>
+      </c>
+      <c r="M139" s="2"/>
+      <c r="N139" s="2">
+        <v>0.47513532638549799</v>
+      </c>
+      <c r="O139" s="2"/>
+      <c r="P139" s="2">
+        <v>0.470775017264912</v>
+      </c>
+      <c r="Q139" s="2"/>
+      <c r="R139" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S139" s="2"/>
+    </row>
+    <row r="140" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C140">
+        <f t="shared" si="0"/>
+        <v>3.2927999818757304E-3</v>
+      </c>
+      <c r="D140" s="2">
+        <v>0.97744923830032304</v>
+      </c>
+      <c r="E140" s="2"/>
+      <c r="F140" s="2">
+        <v>0.97748142480850198</v>
+      </c>
+      <c r="G140" s="2"/>
+      <c r="H140" s="2"/>
+      <c r="L140" s="2"/>
+      <c r="M140" s="2"/>
+      <c r="N140" s="2"/>
+      <c r="O140" s="2"/>
+      <c r="P140" s="2"/>
+      <c r="Q140" s="2"/>
+      <c r="R140" s="2"/>
+      <c r="S140" s="2"/>
+    </row>
+    <row r="141" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C141">
+        <f t="shared" si="0"/>
+        <v>3.4668222668214929E-3</v>
+      </c>
+      <c r="D141" s="2">
+        <v>0.97652149200439398</v>
+      </c>
+      <c r="E141" s="2"/>
+      <c r="F141" s="2">
+        <v>0.97655534744262695</v>
+      </c>
+      <c r="G141" s="2"/>
+      <c r="H141" s="2"/>
+      <c r="L141" s="2"/>
+      <c r="M141" s="2"/>
+      <c r="N141" s="2"/>
+      <c r="O141" s="2"/>
+      <c r="P141" s="2"/>
+      <c r="Q141" s="2"/>
+      <c r="R141" s="2"/>
+      <c r="S141" s="2"/>
+    </row>
+    <row r="142" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C142">
+        <f t="shared" si="0"/>
+        <v>5.3130239338508925E-3</v>
+      </c>
+      <c r="D142" s="2">
+        <v>0.97820919752120905</v>
+      </c>
+      <c r="E142" s="2"/>
+      <c r="F142" s="2">
+        <v>0.97826117277145397</v>
+      </c>
+      <c r="G142" s="2"/>
+      <c r="H142" s="2"/>
+      <c r="L142" s="2"/>
+      <c r="M142" s="2"/>
+      <c r="N142" s="2"/>
+      <c r="O142" s="2"/>
+      <c r="P142" s="2"/>
+      <c r="Q142" s="2"/>
+      <c r="R142" s="2"/>
+      <c r="S142" s="2"/>
+    </row>
+    <row r="143" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C143">
+        <f t="shared" si="0"/>
+        <v>1.4718673214026241E-2</v>
+      </c>
+      <c r="D143" s="2">
+        <v>-0.97823780775070102</v>
+      </c>
+      <c r="E143" s="2"/>
+      <c r="F143" s="2">
+        <v>-0.97838181257247903</v>
+      </c>
+      <c r="G143" s="2"/>
+      <c r="H143" s="2"/>
+      <c r="L143" s="2"/>
+      <c r="M143" s="2"/>
+      <c r="N143" s="2"/>
+      <c r="O143" s="2"/>
+      <c r="P143" s="2"/>
+      <c r="Q143" s="2"/>
+      <c r="R143" s="2"/>
+      <c r="S143" s="2"/>
+    </row>
+    <row r="144" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C144">
+        <f t="shared" si="0"/>
+        <v>6.4173831933433114E-3</v>
+      </c>
+      <c r="D144" s="2">
+        <v>0.97889220714569003</v>
+      </c>
+      <c r="E144" s="2"/>
+      <c r="F144" s="2">
+        <v>0.97895503044128396</v>
+      </c>
+      <c r="G144" s="2"/>
+      <c r="H144" s="2"/>
+      <c r="L144" s="2"/>
+      <c r="M144" s="2"/>
+      <c r="N144" s="2"/>
+      <c r="O144" s="2"/>
+      <c r="P144" s="2"/>
+      <c r="Q144" s="2"/>
+      <c r="R144" s="2"/>
+      <c r="S144" s="2"/>
+    </row>
+    <row r="145" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C145">
+        <f t="shared" si="0"/>
+        <v>2.9992141693686311E-3</v>
+      </c>
+      <c r="D145" s="2">
+        <v>0.97774296998977595</v>
+      </c>
+      <c r="E145" s="2"/>
+      <c r="F145" s="2">
+        <v>0.97777229547500599</v>
+      </c>
+      <c r="G145" s="2"/>
+      <c r="H145" s="2"/>
+      <c r="L145" s="2"/>
+      <c r="M145" s="2"/>
+      <c r="N145" s="2"/>
+      <c r="O145" s="2"/>
+      <c r="P145" s="2"/>
+      <c r="Q145" s="2"/>
+      <c r="R145" s="2"/>
+      <c r="S145" s="2"/>
+    </row>
+    <row r="146" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C146">
+        <f t="shared" si="0"/>
+        <v>6.8079897448530217E-3</v>
+      </c>
+      <c r="D146" s="2">
+        <v>0.97962921857833796</v>
+      </c>
+      <c r="E146" s="2"/>
+      <c r="F146" s="2">
+        <v>0.97969591617584195</v>
+      </c>
+      <c r="G146" s="2"/>
+      <c r="H146" s="2"/>
+      <c r="L146" s="2"/>
+      <c r="M146" s="2"/>
+      <c r="N146" s="2"/>
+      <c r="O146" s="2"/>
+      <c r="P146" s="2"/>
+      <c r="Q146" s="2"/>
+      <c r="R146" s="2"/>
+      <c r="S146" s="2"/>
+    </row>
+    <row r="147" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C147">
+        <f t="shared" si="0"/>
+        <v>5.8598248277854162E-3</v>
+      </c>
+      <c r="D147" s="2">
+        <v>0.97846454381942705</v>
+      </c>
+      <c r="E147" s="2"/>
+      <c r="F147" s="2">
+        <v>0.97852188348770097</v>
+      </c>
+      <c r="G147" s="2"/>
+      <c r="H147" s="2"/>
+      <c r="L147" s="2"/>
+      <c r="M147" s="2"/>
+      <c r="N147" s="2"/>
+      <c r="O147" s="2"/>
+      <c r="P147" s="2"/>
+      <c r="Q147" s="2"/>
+      <c r="R147" s="2"/>
+      <c r="S147" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="212">
+  <mergeCells count="314">
+    <mergeCell ref="C119:C120"/>
+    <mergeCell ref="L112:M120"/>
+    <mergeCell ref="L121:M129"/>
+    <mergeCell ref="L130:M138"/>
+    <mergeCell ref="L139:M147"/>
+    <mergeCell ref="N130:O138"/>
+    <mergeCell ref="P130:Q138"/>
+    <mergeCell ref="R130:S138"/>
+    <mergeCell ref="N139:O147"/>
+    <mergeCell ref="P139:Q147"/>
+    <mergeCell ref="R139:S147"/>
+    <mergeCell ref="N112:O120"/>
+    <mergeCell ref="P112:Q120"/>
+    <mergeCell ref="R112:S120"/>
+    <mergeCell ref="N121:O129"/>
+    <mergeCell ref="P121:Q129"/>
+    <mergeCell ref="R121:S129"/>
+    <mergeCell ref="C109:G109"/>
+    <mergeCell ref="R110:S111"/>
+    <mergeCell ref="N111:O111"/>
+    <mergeCell ref="P111:Q111"/>
+    <mergeCell ref="L110:Q110"/>
+    <mergeCell ref="L111:M111"/>
+    <mergeCell ref="F139:G139"/>
+    <mergeCell ref="H139:H147"/>
+    <mergeCell ref="F140:G140"/>
+    <mergeCell ref="F141:G141"/>
+    <mergeCell ref="D142:E142"/>
+    <mergeCell ref="F142:G142"/>
+    <mergeCell ref="D143:E143"/>
+    <mergeCell ref="F143:G143"/>
+    <mergeCell ref="D144:E144"/>
+    <mergeCell ref="F144:G144"/>
+    <mergeCell ref="D145:E145"/>
+    <mergeCell ref="F145:G145"/>
+    <mergeCell ref="D146:E146"/>
+    <mergeCell ref="F146:G146"/>
+    <mergeCell ref="D147:E147"/>
+    <mergeCell ref="F147:G147"/>
+    <mergeCell ref="F130:G130"/>
+    <mergeCell ref="H130:H138"/>
+    <mergeCell ref="F131:G131"/>
+    <mergeCell ref="F132:G132"/>
+    <mergeCell ref="F133:G133"/>
+    <mergeCell ref="F134:G134"/>
+    <mergeCell ref="F135:G135"/>
+    <mergeCell ref="F136:G136"/>
+    <mergeCell ref="F137:G137"/>
+    <mergeCell ref="F138:G138"/>
+    <mergeCell ref="F119:G120"/>
+    <mergeCell ref="F121:G121"/>
+    <mergeCell ref="H121:H129"/>
+    <mergeCell ref="F122:G122"/>
+    <mergeCell ref="F123:G123"/>
+    <mergeCell ref="F124:G124"/>
+    <mergeCell ref="F125:G125"/>
+    <mergeCell ref="F126:G126"/>
+    <mergeCell ref="F127:G127"/>
+    <mergeCell ref="F128:G128"/>
+    <mergeCell ref="F129:G129"/>
+    <mergeCell ref="D141:E141"/>
+    <mergeCell ref="H109:H110"/>
+    <mergeCell ref="F110:G110"/>
+    <mergeCell ref="F111:G111"/>
+    <mergeCell ref="H111:H120"/>
+    <mergeCell ref="F112:G112"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="F113:G113"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="F114:G114"/>
+    <mergeCell ref="F115:G115"/>
+    <mergeCell ref="F116:G116"/>
+    <mergeCell ref="F117:G117"/>
+    <mergeCell ref="F118:G118"/>
+    <mergeCell ref="D119:E120"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="D135:E135"/>
+    <mergeCell ref="D136:E136"/>
+    <mergeCell ref="D137:E137"/>
+    <mergeCell ref="D138:E138"/>
+    <mergeCell ref="D139:E139"/>
+    <mergeCell ref="D140:E140"/>
+    <mergeCell ref="D131:E131"/>
+    <mergeCell ref="D132:E132"/>
+    <mergeCell ref="D133:E133"/>
+    <mergeCell ref="D123:E123"/>
+    <mergeCell ref="D124:E124"/>
+    <mergeCell ref="D125:E125"/>
+    <mergeCell ref="D126:E126"/>
+    <mergeCell ref="D127:E127"/>
+    <mergeCell ref="D128:E128"/>
+    <mergeCell ref="D129:E129"/>
+    <mergeCell ref="D130:E130"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="D117:E117"/>
+    <mergeCell ref="D118:E118"/>
+    <mergeCell ref="D121:E121"/>
+    <mergeCell ref="D122:E122"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="D111:E111"/>
     <mergeCell ref="P58:R58"/>
     <mergeCell ref="S58:T58"/>
     <mergeCell ref="P59:R59"/>

</xml_diff>

<commit_message>
fix: datas in excel
</commit_message>
<xml_diff>
--- a/Simulasi_Vector/Weight dan bias hasil training.xlsx
+++ b/Simulasi_Vector/Weight dan bias hasil training.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Okinawa\UAS_VLSI_LEVEL1-OKINAWA\Simulasi_Vector\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Falih\VLSI\UAS_VLSI_LEVEL1-OKINAWA\Simulasi_Vector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACDD67F-DD65-43AB-815B-3D8808CAEA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0DBFEA9-CD08-455B-A944-6D368E77C2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C54F6822-D4A8-46D5-BD9B-B2A846AAD251}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{C54F6822-D4A8-46D5-BD9B-B2A846AAD251}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0.000000000000000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.000000000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -150,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -158,8 +158,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -180,9 +179,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -220,7 +219,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -326,7 +325,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -468,7 +467,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -478,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05913C57-9BC5-4BEF-9885-2849EB63E124}">
   <dimension ref="A1:T147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="63" workbookViewId="0">
-      <selection activeCell="J123" sqref="J123"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="63" workbookViewId="0">
+      <selection activeCell="C109" sqref="C109:S147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1140,11 +1139,11 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
-      <c r="P41" s="4">
+      <c r="P41" s="3">
         <v>0.470764938554386</v>
       </c>
-      <c r="Q41" s="4"/>
-      <c r="R41" s="4"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
       <c r="S41" s="2" t="s">
         <v>13</v>
       </c>
@@ -1174,11 +1173,11 @@
         <v>13</v>
       </c>
       <c r="M42" s="2"/>
-      <c r="P42" s="4">
+      <c r="P42" s="3">
         <v>0.47107202254688402</v>
       </c>
-      <c r="Q42" s="4"/>
-      <c r="R42" s="4"/>
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3"/>
       <c r="S42" s="2" t="s">
         <v>14</v>
       </c>
@@ -1277,11 +1276,11 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
-      <c r="P47" s="4">
+      <c r="P47" s="3">
         <v>0.470996508933822</v>
       </c>
-      <c r="Q47" s="4"/>
-      <c r="R47" s="4"/>
+      <c r="Q47" s="3"/>
+      <c r="R47" s="3"/>
       <c r="S47" s="2" t="s">
         <v>16</v>
       </c>
@@ -1303,11 +1302,11 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
-      <c r="P48" s="4">
+      <c r="P48" s="3">
         <v>0.47080308116633002</v>
       </c>
-      <c r="Q48" s="4"/>
-      <c r="R48" s="4"/>
+      <c r="Q48" s="3"/>
+      <c r="R48" s="3"/>
       <c r="S48" s="2" t="s">
         <v>17</v>
       </c>
@@ -1393,11 +1392,11 @@
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
-      <c r="P52" s="4">
+      <c r="P52" s="3">
         <v>0.467146543573427</v>
       </c>
-      <c r="Q52" s="4"/>
-      <c r="R52" s="4"/>
+      <c r="Q52" s="3"/>
+      <c r="R52" s="3"/>
       <c r="S52" s="2" t="s">
         <v>13</v>
       </c>
@@ -1419,11 +1418,11 @@
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
-      <c r="P53" s="4">
+      <c r="P53" s="3">
         <v>0.46739828818349</v>
       </c>
-      <c r="Q53" s="4"/>
-      <c r="R53" s="4"/>
+      <c r="Q53" s="3"/>
+      <c r="R53" s="3"/>
       <c r="S53" s="2" t="s">
         <v>14</v>
       </c>
@@ -1522,11 +1521,11 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
-      <c r="P58" s="4">
+      <c r="P58" s="3">
         <v>0.47087036808694599</v>
       </c>
-      <c r="Q58" s="4"/>
-      <c r="R58" s="4"/>
+      <c r="Q58" s="3"/>
+      <c r="R58" s="3"/>
       <c r="S58" s="2" t="s">
         <v>16</v>
       </c>
@@ -1548,11 +1547,11 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
-      <c r="P59" s="4">
+      <c r="P59" s="3">
         <v>0.470775017264912</v>
       </c>
-      <c r="Q59" s="4"/>
-      <c r="R59" s="4"/>
+      <c r="Q59" s="3"/>
+      <c r="R59" s="3"/>
       <c r="S59" s="2" t="s">
         <v>17</v>
       </c>
@@ -2177,10 +2176,6 @@
       <c r="S91" s="2"/>
       <c r="T91" s="2"/>
     </row>
-    <row r="92" spans="3:20" x14ac:dyDescent="0.35">
-      <c r="C92" s="3"/>
-      <c r="D92" s="3"/>
-    </row>
     <row r="93" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C93" s="2" t="s">
         <v>20</v>
@@ -2466,10 +2461,6 @@
       <c r="R102" s="2"/>
       <c r="S102" s="2"/>
       <c r="T102" s="2"/>
-    </row>
-    <row r="103" spans="3:20" x14ac:dyDescent="0.35">
-      <c r="C103" s="3"/>
-      <c r="D103" s="3"/>
     </row>
     <row r="109" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C109" s="2" t="s">
@@ -3405,23 +3396,272 @@
     </row>
   </sheetData>
   <mergeCells count="314">
-    <mergeCell ref="C119:C120"/>
-    <mergeCell ref="L112:M120"/>
-    <mergeCell ref="L121:M129"/>
-    <mergeCell ref="L130:M138"/>
-    <mergeCell ref="L139:M147"/>
-    <mergeCell ref="N130:O138"/>
-    <mergeCell ref="P130:Q138"/>
-    <mergeCell ref="R130:S138"/>
-    <mergeCell ref="N139:O147"/>
-    <mergeCell ref="P139:Q147"/>
-    <mergeCell ref="R139:S147"/>
-    <mergeCell ref="N112:O120"/>
-    <mergeCell ref="P112:Q120"/>
-    <mergeCell ref="R112:S120"/>
-    <mergeCell ref="N121:O129"/>
-    <mergeCell ref="P121:Q129"/>
-    <mergeCell ref="R121:S129"/>
+    <mergeCell ref="H40:K40"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="L40:M41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="F42:F51"/>
+    <mergeCell ref="F52:F60"/>
+    <mergeCell ref="F61:F69"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="L69:M77"/>
+    <mergeCell ref="L60:M68"/>
+    <mergeCell ref="H51:I59"/>
+    <mergeCell ref="J51:K59"/>
+    <mergeCell ref="L42:M50"/>
+    <mergeCell ref="L51:M59"/>
+    <mergeCell ref="H42:I50"/>
+    <mergeCell ref="J42:K50"/>
+    <mergeCell ref="F70:F78"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="H60:I68"/>
+    <mergeCell ref="J60:K68"/>
+    <mergeCell ref="H69:I77"/>
+    <mergeCell ref="J69:K77"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="B50:C51"/>
+    <mergeCell ref="D50:E51"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="E83:E91"/>
+    <mergeCell ref="I83:I91"/>
+    <mergeCell ref="F87:H87"/>
+    <mergeCell ref="F88:H88"/>
+    <mergeCell ref="F89:H89"/>
+    <mergeCell ref="F90:H90"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="P91:R91"/>
+    <mergeCell ref="K86:M86"/>
+    <mergeCell ref="K87:M87"/>
+    <mergeCell ref="K88:M88"/>
+    <mergeCell ref="K89:M89"/>
+    <mergeCell ref="K85:M85"/>
+    <mergeCell ref="S82:T82"/>
+    <mergeCell ref="S83:T91"/>
+    <mergeCell ref="N82:O82"/>
+    <mergeCell ref="N83:O91"/>
+    <mergeCell ref="K82:M82"/>
+    <mergeCell ref="K83:M83"/>
+    <mergeCell ref="K84:M84"/>
+    <mergeCell ref="P82:R82"/>
+    <mergeCell ref="P83:R83"/>
+    <mergeCell ref="P84:R84"/>
+    <mergeCell ref="P85:R85"/>
+    <mergeCell ref="P86:R86"/>
+    <mergeCell ref="P87:R87"/>
+    <mergeCell ref="P88:R88"/>
+    <mergeCell ref="P89:R89"/>
+    <mergeCell ref="P90:R90"/>
+    <mergeCell ref="P42:R42"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="P46:R46"/>
+    <mergeCell ref="S46:T46"/>
+    <mergeCell ref="P47:R47"/>
+    <mergeCell ref="S47:T47"/>
+    <mergeCell ref="P40:R40"/>
+    <mergeCell ref="S40:T40"/>
+    <mergeCell ref="P41:R41"/>
+    <mergeCell ref="S41:T41"/>
+    <mergeCell ref="P48:R48"/>
+    <mergeCell ref="S48:T48"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="F93:H93"/>
+    <mergeCell ref="K93:M93"/>
+    <mergeCell ref="N93:O93"/>
+    <mergeCell ref="P93:R93"/>
+    <mergeCell ref="S93:T93"/>
+    <mergeCell ref="P51:R51"/>
+    <mergeCell ref="S51:T51"/>
+    <mergeCell ref="P52:R52"/>
+    <mergeCell ref="S52:T52"/>
+    <mergeCell ref="P53:R53"/>
+    <mergeCell ref="S53:T53"/>
+    <mergeCell ref="P57:R57"/>
+    <mergeCell ref="S57:T57"/>
+    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="F83:H83"/>
+    <mergeCell ref="F84:H84"/>
+    <mergeCell ref="F85:H85"/>
+    <mergeCell ref="F86:H86"/>
+    <mergeCell ref="F82:H82"/>
+    <mergeCell ref="K90:M90"/>
+    <mergeCell ref="K91:M91"/>
+    <mergeCell ref="K96:M96"/>
+    <mergeCell ref="P96:R96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="F97:H97"/>
+    <mergeCell ref="K97:M97"/>
+    <mergeCell ref="P97:R97"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="E94:E102"/>
+    <mergeCell ref="F94:H94"/>
+    <mergeCell ref="I94:I102"/>
+    <mergeCell ref="K94:M94"/>
+    <mergeCell ref="F98:H98"/>
+    <mergeCell ref="K98:M98"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="F100:H100"/>
+    <mergeCell ref="K100:M100"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="F102:H102"/>
+    <mergeCell ref="K102:M102"/>
+    <mergeCell ref="P58:R58"/>
+    <mergeCell ref="S58:T58"/>
+    <mergeCell ref="P59:R59"/>
+    <mergeCell ref="S59:T59"/>
+    <mergeCell ref="P102:R102"/>
+    <mergeCell ref="P100:R100"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="F101:H101"/>
+    <mergeCell ref="K101:M101"/>
+    <mergeCell ref="P101:R101"/>
+    <mergeCell ref="P98:R98"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="F99:H99"/>
+    <mergeCell ref="K99:M99"/>
+    <mergeCell ref="P99:R99"/>
+    <mergeCell ref="N94:O102"/>
+    <mergeCell ref="P94:R94"/>
+    <mergeCell ref="S94:T102"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="F95:H95"/>
+    <mergeCell ref="K95:M95"/>
+    <mergeCell ref="P95:R95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="F96:H96"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="D117:E117"/>
+    <mergeCell ref="D118:E118"/>
+    <mergeCell ref="D121:E121"/>
+    <mergeCell ref="D122:E122"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="D133:E133"/>
+    <mergeCell ref="D123:E123"/>
+    <mergeCell ref="D124:E124"/>
+    <mergeCell ref="D125:E125"/>
+    <mergeCell ref="D126:E126"/>
+    <mergeCell ref="D127:E127"/>
+    <mergeCell ref="D128:E128"/>
+    <mergeCell ref="D129:E129"/>
+    <mergeCell ref="D130:E130"/>
+    <mergeCell ref="D141:E141"/>
+    <mergeCell ref="H109:H110"/>
+    <mergeCell ref="F110:G110"/>
+    <mergeCell ref="F111:G111"/>
+    <mergeCell ref="H111:H120"/>
+    <mergeCell ref="F112:G112"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="F113:G113"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="F114:G114"/>
+    <mergeCell ref="F115:G115"/>
+    <mergeCell ref="F116:G116"/>
+    <mergeCell ref="F117:G117"/>
+    <mergeCell ref="F118:G118"/>
+    <mergeCell ref="D119:E120"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="D135:E135"/>
+    <mergeCell ref="D136:E136"/>
+    <mergeCell ref="D137:E137"/>
+    <mergeCell ref="D138:E138"/>
+    <mergeCell ref="D139:E139"/>
+    <mergeCell ref="D140:E140"/>
+    <mergeCell ref="D131:E131"/>
+    <mergeCell ref="D132:E132"/>
+    <mergeCell ref="F138:G138"/>
+    <mergeCell ref="F119:G120"/>
+    <mergeCell ref="F121:G121"/>
+    <mergeCell ref="H121:H129"/>
+    <mergeCell ref="F122:G122"/>
+    <mergeCell ref="F123:G123"/>
+    <mergeCell ref="F124:G124"/>
+    <mergeCell ref="F125:G125"/>
+    <mergeCell ref="F126:G126"/>
+    <mergeCell ref="F127:G127"/>
+    <mergeCell ref="F128:G128"/>
+    <mergeCell ref="F129:G129"/>
     <mergeCell ref="C109:G109"/>
     <mergeCell ref="R110:S111"/>
     <mergeCell ref="N111:O111"/>
@@ -3446,6 +3686,23 @@
     <mergeCell ref="F147:G147"/>
     <mergeCell ref="F130:G130"/>
     <mergeCell ref="H130:H138"/>
+    <mergeCell ref="C119:C120"/>
+    <mergeCell ref="L112:M120"/>
+    <mergeCell ref="L121:M129"/>
+    <mergeCell ref="L130:M138"/>
+    <mergeCell ref="L139:M147"/>
+    <mergeCell ref="N130:O138"/>
+    <mergeCell ref="P130:Q138"/>
+    <mergeCell ref="R130:S138"/>
+    <mergeCell ref="N139:O147"/>
+    <mergeCell ref="P139:Q147"/>
+    <mergeCell ref="R139:S147"/>
+    <mergeCell ref="N112:O120"/>
+    <mergeCell ref="P112:Q120"/>
+    <mergeCell ref="R112:S120"/>
+    <mergeCell ref="N121:O129"/>
+    <mergeCell ref="P121:Q129"/>
+    <mergeCell ref="R121:S129"/>
     <mergeCell ref="F131:G131"/>
     <mergeCell ref="F132:G132"/>
     <mergeCell ref="F133:G133"/>
@@ -3453,272 +3710,6 @@
     <mergeCell ref="F135:G135"/>
     <mergeCell ref="F136:G136"/>
     <mergeCell ref="F137:G137"/>
-    <mergeCell ref="F138:G138"/>
-    <mergeCell ref="F119:G120"/>
-    <mergeCell ref="F121:G121"/>
-    <mergeCell ref="H121:H129"/>
-    <mergeCell ref="F122:G122"/>
-    <mergeCell ref="F123:G123"/>
-    <mergeCell ref="F124:G124"/>
-    <mergeCell ref="F125:G125"/>
-    <mergeCell ref="F126:G126"/>
-    <mergeCell ref="F127:G127"/>
-    <mergeCell ref="F128:G128"/>
-    <mergeCell ref="F129:G129"/>
-    <mergeCell ref="D141:E141"/>
-    <mergeCell ref="H109:H110"/>
-    <mergeCell ref="F110:G110"/>
-    <mergeCell ref="F111:G111"/>
-    <mergeCell ref="H111:H120"/>
-    <mergeCell ref="F112:G112"/>
-    <mergeCell ref="D113:E113"/>
-    <mergeCell ref="F113:G113"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="F114:G114"/>
-    <mergeCell ref="F115:G115"/>
-    <mergeCell ref="F116:G116"/>
-    <mergeCell ref="F117:G117"/>
-    <mergeCell ref="F118:G118"/>
-    <mergeCell ref="D119:E120"/>
-    <mergeCell ref="D134:E134"/>
-    <mergeCell ref="D135:E135"/>
-    <mergeCell ref="D136:E136"/>
-    <mergeCell ref="D137:E137"/>
-    <mergeCell ref="D138:E138"/>
-    <mergeCell ref="D139:E139"/>
-    <mergeCell ref="D140:E140"/>
-    <mergeCell ref="D131:E131"/>
-    <mergeCell ref="D132:E132"/>
-    <mergeCell ref="D133:E133"/>
-    <mergeCell ref="D123:E123"/>
-    <mergeCell ref="D124:E124"/>
-    <mergeCell ref="D125:E125"/>
-    <mergeCell ref="D126:E126"/>
-    <mergeCell ref="D127:E127"/>
-    <mergeCell ref="D128:E128"/>
-    <mergeCell ref="D129:E129"/>
-    <mergeCell ref="D130:E130"/>
-    <mergeCell ref="D116:E116"/>
-    <mergeCell ref="D117:E117"/>
-    <mergeCell ref="D118:E118"/>
-    <mergeCell ref="D121:E121"/>
-    <mergeCell ref="D122:E122"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="P58:R58"/>
-    <mergeCell ref="S58:T58"/>
-    <mergeCell ref="P59:R59"/>
-    <mergeCell ref="S59:T59"/>
-    <mergeCell ref="P102:R102"/>
-    <mergeCell ref="P100:R100"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="F101:H101"/>
-    <mergeCell ref="K101:M101"/>
-    <mergeCell ref="P101:R101"/>
-    <mergeCell ref="P98:R98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="F99:H99"/>
-    <mergeCell ref="K99:M99"/>
-    <mergeCell ref="P99:R99"/>
-    <mergeCell ref="N94:O102"/>
-    <mergeCell ref="P94:R94"/>
-    <mergeCell ref="S94:T102"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="F95:H95"/>
-    <mergeCell ref="K95:M95"/>
-    <mergeCell ref="P95:R95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="F96:H96"/>
-    <mergeCell ref="K96:M96"/>
-    <mergeCell ref="P96:R96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="F97:H97"/>
-    <mergeCell ref="K97:M97"/>
-    <mergeCell ref="P97:R97"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="E94:E102"/>
-    <mergeCell ref="F94:H94"/>
-    <mergeCell ref="I94:I102"/>
-    <mergeCell ref="K94:M94"/>
-    <mergeCell ref="F98:H98"/>
-    <mergeCell ref="K98:M98"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="F100:H100"/>
-    <mergeCell ref="K100:M100"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="F102:H102"/>
-    <mergeCell ref="K102:M102"/>
-    <mergeCell ref="P48:R48"/>
-    <mergeCell ref="S48:T48"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="F93:H93"/>
-    <mergeCell ref="K93:M93"/>
-    <mergeCell ref="N93:O93"/>
-    <mergeCell ref="P93:R93"/>
-    <mergeCell ref="S93:T93"/>
-    <mergeCell ref="P51:R51"/>
-    <mergeCell ref="S51:T51"/>
-    <mergeCell ref="P52:R52"/>
-    <mergeCell ref="S52:T52"/>
-    <mergeCell ref="P53:R53"/>
-    <mergeCell ref="S53:T53"/>
-    <mergeCell ref="P57:R57"/>
-    <mergeCell ref="S57:T57"/>
-    <mergeCell ref="P42:R42"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="P46:R46"/>
-    <mergeCell ref="S46:T46"/>
-    <mergeCell ref="P47:R47"/>
-    <mergeCell ref="S47:T47"/>
-    <mergeCell ref="P40:R40"/>
-    <mergeCell ref="S40:T40"/>
-    <mergeCell ref="P41:R41"/>
-    <mergeCell ref="S41:T41"/>
-    <mergeCell ref="F91:H91"/>
-    <mergeCell ref="F83:H83"/>
-    <mergeCell ref="F84:H84"/>
-    <mergeCell ref="F85:H85"/>
-    <mergeCell ref="F86:H86"/>
-    <mergeCell ref="F82:H82"/>
-    <mergeCell ref="K90:M90"/>
-    <mergeCell ref="K91:M91"/>
-    <mergeCell ref="P82:R82"/>
-    <mergeCell ref="P83:R83"/>
-    <mergeCell ref="P84:R84"/>
-    <mergeCell ref="P85:R85"/>
-    <mergeCell ref="P86:R86"/>
-    <mergeCell ref="P87:R87"/>
-    <mergeCell ref="P88:R88"/>
-    <mergeCell ref="P89:R89"/>
-    <mergeCell ref="P90:R90"/>
-    <mergeCell ref="P91:R91"/>
-    <mergeCell ref="K86:M86"/>
-    <mergeCell ref="K87:M87"/>
-    <mergeCell ref="K88:M88"/>
-    <mergeCell ref="K89:M89"/>
-    <mergeCell ref="K85:M85"/>
-    <mergeCell ref="S82:T82"/>
-    <mergeCell ref="S83:T91"/>
-    <mergeCell ref="N82:O82"/>
-    <mergeCell ref="N83:O91"/>
-    <mergeCell ref="K82:M82"/>
-    <mergeCell ref="K83:M83"/>
-    <mergeCell ref="K84:M84"/>
-    <mergeCell ref="E83:E91"/>
-    <mergeCell ref="I83:I91"/>
-    <mergeCell ref="F87:H87"/>
-    <mergeCell ref="F88:H88"/>
-    <mergeCell ref="F89:H89"/>
-    <mergeCell ref="F90:H90"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="B50:C51"/>
-    <mergeCell ref="D50:E51"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="H60:I68"/>
-    <mergeCell ref="J60:K68"/>
-    <mergeCell ref="H69:I77"/>
-    <mergeCell ref="J69:K77"/>
-    <mergeCell ref="L69:M77"/>
-    <mergeCell ref="L60:M68"/>
-    <mergeCell ref="H51:I59"/>
-    <mergeCell ref="J51:K59"/>
-    <mergeCell ref="L42:M50"/>
-    <mergeCell ref="L51:M59"/>
-    <mergeCell ref="H42:I50"/>
-    <mergeCell ref="J42:K50"/>
-    <mergeCell ref="F70:F78"/>
-    <mergeCell ref="H40:K40"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="L40:M41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="F42:F51"/>
-    <mergeCell ref="F52:F60"/>
-    <mergeCell ref="F61:F69"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>